<commit_message>
Lab Tests - Lipid Profile -Third Scenario
</commit_message>
<xml_diff>
--- a/Practo/src/test/resources/Excel/PractoTestSc1.xlsx
+++ b/Practo/src/test/resources/Excel/PractoTestSc1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\training\java\SprintPracto\Practo\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{840D3777-7E95-4FFE-A774-BC26340C80D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BAEDA5-AC58-40CA-AB54-8EDA24B96323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{39B25D9C-F411-4BCB-9A7E-8020505F5A5B}"/>
+    <workbookView xWindow="4800" yWindow="1460" windowWidth="14400" windowHeight="9820" xr2:uid="{39B25D9C-F411-4BCB-9A7E-8020505F5A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,30 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>URL</t>
+    <t>HDL</t>
   </si>
   <si>
-    <t>Expected Behavior</t>
+    <t>Cholesterol</t>
   </si>
   <si>
-    <t>https://www.practo.com</t>
+    <t>Lipid Test</t>
   </si>
   <si>
-    <t>Homepage should open</t>
-  </si>
-  <si>
-    <t>https://www.practo.com/tests?city=bangalore</t>
-  </si>
-  <si>
-    <t>Lab Tests page should open</t>
-  </si>
-  <si>
-    <t>https://www.practo.com/tests/lipid-profile-blood/p?city=bangalore</t>
-  </si>
-  <si>
-    <t>Should navigate to test page</t>
+    <t>TestName</t>
   </si>
 </sst>
 </file>
@@ -97,7 +85,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC7E628-4130-4CFA-AFB5-5FBB19F150F3}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -443,36 +433,24 @@
     <col min="1" max="2" width="40.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>